<commit_message>
I think it's done :O
</commit_message>
<xml_diff>
--- a/Conversao.xlsx
+++ b/Conversao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ISEL\3º Semestre\FSO\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\JAVA\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{9E1C3B6C-541B-459A-B059-E68B78DB4EE4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65837B77-AE02-44C3-8DF6-8F0C0F0B1681}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" xr2:uid="{4A797ECC-2AC1-47CA-B2C9-6C161BA17D86}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>%</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Conversão tempo/distancia</t>
   </si>
   <si>
-    <t>Conversão</t>
+    <t>Anda</t>
   </si>
 </sst>
 </file>
@@ -242,24 +242,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -278,6 +266,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,7 +300,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -592,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799C44CB-93DA-4C7B-90A2-304694FDBDCE}">
-  <dimension ref="D4:J13"/>
+  <dimension ref="D4:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,101 +608,208 @@
     <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="4" t="s">
+    <row r="4" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="4" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="7" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="7">
+    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
         <v>50</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.2</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="H7" s="7">
+      <c r="F7" s="5"/>
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f>E8</f>
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="6">
+        <v>75</v>
+      </c>
+      <c r="E8" s="7">
+        <f>D8*E7/D7</f>
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="8">
+        <f>E8*100</f>
+        <v>30</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <f>H8*I7/H7</f>
+        <v>0.3</v>
+      </c>
+      <c r="J8" s="8">
+        <f>I8*100</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="K11">
         <v>50</v>
       </c>
-      <c r="E8" s="11">
-        <f>D8*E7/D7</f>
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="12">
-        <f>E8*100</f>
+      <c r="L11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="10">
-        <v>5</v>
-      </c>
-      <c r="I8" s="11">
-        <f>H8*I7/H7</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="12">
-        <f>I8*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
-        <v>2</v>
-      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>30</v>
+      </c>
+      <c r="E14" s="1">
+        <v>60</v>
+      </c>
+      <c r="F14" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1">
+        <v>28</v>
+      </c>
+      <c r="K16">
+        <f>((K12-K11)/(K13-K11))*(L13-L11)+L11</f>
+        <v>62.5</v>
+      </c>
+      <c r="N16">
+        <f>(K12-K11)/(K13-K11)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>